<commit_message>
Addition of data to CiLVpUAAbP and CSpULApYbP
- CSpULApYbP: Forest Set Aside -> No data
- CSpULApYbP: Figures more consistent except peatland restoration
- CiLVpUAAbP: Incomplete, stuggled to find complete info
</commit_message>
<xml_diff>
--- a/InputData/land/CSpULApYbP/CO2 Sequestered per Unit Land Area per Year by Pol.xlsx
+++ b/InputData/land/CSpULApYbP/CO2 Sequestered per Unit Land Area per Year by Pol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anima\Desktop\Models\eps-brazil-cpl\InputData\land\CSpULApYbP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anima\OneDrive\Desktop\Models\eps-brazil-cpl2\InputData\land\CSpULApYbP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995164BC-836C-4A11-9078-520056A0CEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16394AB-C966-454E-8DBE-D40E2A3AA1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -67,12 +67,25 @@
     <definedName name="N2O_to_CO2e">'[2]Cross-Page Data'!$C$13</definedName>
     <definedName name="unit_conv">[7]About!$A$111</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>CSpULApYbP CO2 Sequestered per Unit Land Area per Year by Policy</t>
   </si>
@@ -218,20 +231,65 @@
     <t>kg/ha/yr</t>
   </si>
   <si>
-    <t>kg/acre/yr</t>
+    <t>Peatland Restoration</t>
+  </si>
+  <si>
+    <t>UNEP</t>
+  </si>
+  <si>
+    <t>https://www.uncclearn.org/wp-content/uploads/library/PeatCRSM.pdf#:~:text=Investing%20in%20cost%2Deffective%20tropical%20peatland%20conservation%20and,and%20US$11.7%20billion%20more%20for%20restoration%20(</t>
+  </si>
+  <si>
+    <t>Valladares, G. S. (2003). Caracterização de Organossolos, auxílio à sua classificação. Seropédica: Universidade Federal Rural do Rio de Janeiro.</t>
+  </si>
+  <si>
+    <t>acres of Peatlands</t>
+  </si>
+  <si>
+    <t>g/yr</t>
+  </si>
+  <si>
+    <t>Improved Forest Management</t>
+  </si>
+  <si>
+    <t>"Caracterização de Organossolos, auxílio à sua classificação"</t>
+  </si>
+  <si>
+    <t>"Economics of
+Peatlands Conservation, Restoration and Sustainable Management"</t>
+  </si>
+  <si>
+    <t>Annual Mitigation (Mtons/yr) [2021]</t>
+  </si>
+  <si>
+    <t>Ha of Brazilian Peatlands [2003]</t>
+  </si>
+  <si>
+    <t>Improved Tropical Forest Management for Carbon Retention</t>
+  </si>
+  <si>
+    <t>Putz, F. E., Zuidema, P. A., Pinard, M. A., Boot, R. G. A., Sayer, J. A., Sheil, D., ... &amp; Vanclay, J. K. (2008). Improved tropical forest management for carbon retention. PLoS biology, 6(7), e166.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371/journal.pbio.0060166</t>
+  </si>
+  <si>
+    <t>Sequestration via Improved Forestry Practices (tons/ha/yr)</t>
+  </si>
+  <si>
+    <t>Figure provided is a sum of 2 from the source provided. (30 + 7 = 37)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,12 +350,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -382,7 +434,7 @@
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -391,20 +443,14 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="10" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Body: normal cell" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1375,244 +1421,290 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.453125" customWidth="1"/>
-    <col min="2" max="2" width="66.7265625" customWidth="1"/>
-    <col min="3" max="3" width="84.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.46484375" customWidth="1"/>
+    <col min="2" max="2" width="66.73046875" customWidth="1"/>
+    <col min="3" max="3" width="84.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="11"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="10"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
-      <c r="C7" s="12"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
-      <c r="C8" s="10"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="9"/>
-    </row>
-    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="10"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11">
         <v>2022</v>
       </c>
-      <c r="C11" s="11"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="10"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
-      <c r="C14" s="10"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
-      <c r="C15" s="10"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="9"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="10"/>
-    </row>
-    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="B18" s="8" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="11"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="11"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="10"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C23" s="10"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B22" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B23" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B24">
+        <v>2021</v>
+      </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C26" s="10"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B29" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B31" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B33" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B37" s="6"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A47" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A57" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B42">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B58">
         <v>2.4710538149999999</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C58" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B43">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B59">
         <v>1000000</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C59" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B44">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B60">
         <v>1000</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C60" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="6"/>
-      <c r="B57" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5FC1072-E4E3-45CC-9D75-66CC4DD1CBE1}">
-  <dimension ref="A2:H13"/>
+  <dimension ref="A2:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.53125" customWidth="1"/>
+    <col min="13" max="13" width="29.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1622,8 +1714,14 @@
       <c r="G2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="28.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1642,8 +1740,20 @@
       <c r="H4">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4">
+        <v>4.2</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="N4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1663,15 +1773,21 @@
         <v>600</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6">
+        <v>611883</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1685,16 +1801,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="9">
         <f>B4/B5</f>
         <v>42.284196547144759</v>
       </c>
@@ -1712,44 +1828,72 @@
         <f>H4*H5</f>
         <v>54000</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11">
+        <f>K6*About!B58</f>
+        <v>1511995.8214836449</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11">
+        <f>N4*About!B59/About!B58</f>
+        <v>14973368.760890381</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>44</v>
       </c>
       <c r="B12">
-        <f>B11*About!B42/(About!B43)</f>
-        <v>1.0448652519203187E-4</v>
+        <f>B11*About!B59/About!B58</f>
+        <v>17111807.234009899</v>
       </c>
       <c r="D12" t="s">
         <v>44</v>
       </c>
       <c r="E12">
-        <f>E11/About!B43</f>
-        <v>7.9789601456605296E-5</v>
+        <f>E11*About!B59</f>
+        <v>79789601.4566053</v>
       </c>
       <c r="G12" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H12">
-        <f>H11/About!B42</f>
-        <v>21853.024678056234</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <f>H11*About!B60/About!B58</f>
+        <v>21853024.678056233</v>
+      </c>
+      <c r="J12" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12">
+        <f>K4*About!B59</f>
+        <v>4200000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>43</v>
       </c>
       <c r="B13">
         <f>B12/B7</f>
-        <v>1.0448652519203187E-6</v>
+        <v>171118.072340099</v>
       </c>
       <c r="D13" t="s">
         <v>43</v>
       </c>
       <c r="E13">
         <f>E12/E7</f>
-        <v>3.4691131068089261E-6</v>
+        <v>3469113.106808926</v>
+      </c>
+      <c r="J13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13">
+        <f>K12/K11</f>
+        <v>2.7777854543795981</v>
       </c>
     </row>
   </sheetData>
@@ -1765,16 +1909,16 @@
   <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.26953125" customWidth="1"/>
-    <col min="2" max="2" width="16.90625" customWidth="1"/>
+    <col min="1" max="1" width="29.265625" customWidth="1"/>
+    <col min="2" max="2" width="16.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
@@ -1796,7 +1940,7 @@
       <c r="AH1" s="2"/>
       <c r="AJ1" s="2"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1804,13 +1948,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3">
         <f>Data!E13</f>
-        <v>3.4691131068089261E-6</v>
+        <v>3469113.106808926</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1847,21 +1991,22 @@
       <c r="AI3" s="3"/>
       <c r="AJ3" s="3"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+        <f>Data!N11</f>
+        <v>14973368.760890381</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3">
         <f>Data!H12</f>
-        <v>21853.024678056234</v>
+        <v>21853024.678056233</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1898,12 +2043,13 @@
       <c r="AI5" s="3"/>
       <c r="AJ5" s="3"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3">
-        <v>0</v>
+        <f>Data!K13</f>
+        <v>2.7777854543795981</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1940,13 +2086,13 @@
       <c r="AI6" s="3"/>
       <c r="AJ6" s="3"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3">
         <f>Data!B13</f>
-        <v>1.0448652519203187E-6</v>
+        <v>171118.072340099</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>

</xml_diff>

<commit_message>
Update to CiLVpUAAbP and CSpULApYbP
CSpULApYbP complete with the exception of forest set aside.
CiLVpUAAbP incomplete
</commit_message>
<xml_diff>
--- a/InputData/land/CSpULApYbP/CO2 Sequestered per Unit Land Area per Year by Pol.xlsx
+++ b/InputData/land/CSpULApYbP/CO2 Sequestered per Unit Land Area per Year by Pol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anima\OneDrive\Desktop\Models\eps-brazil-cpl2\InputData\land\CSpULApYbP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16394AB-C966-454E-8DBE-D40E2A3AA1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8409BAE2-6E32-4364-B9E1-CE589962BDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -287,7 +287,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -450,7 +450,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Body: normal cell" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1423,8 +1423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1689,8 +1689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5FC1072-E4E3-45CC-9D75-66CC4DD1CBE1}">
   <dimension ref="A2:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1869,8 +1869,8 @@
         <v>53</v>
       </c>
       <c r="K12">
-        <f>K4*About!B59</f>
-        <v>4200000</v>
+        <f>K4*About!B59*1000000</f>
+        <v>4200000000000</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.45">
@@ -1893,7 +1893,7 @@
       </c>
       <c r="K13">
         <f>K12/K11</f>
-        <v>2.7777854543795981</v>
+        <v>2777785.4543795981</v>
       </c>
     </row>
   </sheetData>
@@ -1909,7 +1909,7 @@
   <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="B6" s="3">
         <f>Data!K13</f>
-        <v>2.7777854543795981</v>
+        <v>2777785.4543795981</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>

</xml_diff>